<commit_message>
2017-08-03 23:19:30 everyday last push
</commit_message>
<xml_diff>
--- a/docs/signin_system_dbdisgin.xlsx
+++ b/docs/signin_system_dbdisgin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="9015"/>
+    <workbookView windowWidth="21495" windowHeight="10590"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66">
   <si>
     <t>考研學習記錄，籤到系統</t>
   </si>
@@ -49,6 +49,9 @@
     <t>nickname</t>
   </si>
   <si>
+    <t>created_at</t>
+  </si>
+  <si>
     <t>sign_actions 打卡规则表</t>
   </si>
   <si>
@@ -73,31 +76,37 @@
     <t>開始日期</t>
   </si>
   <si>
+    <t>status_del</t>
+  </si>
+  <si>
+    <t>0--del</t>
+  </si>
+  <si>
     <t>end_time</t>
   </si>
   <si>
     <t>結束日期</t>
   </si>
   <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>week_set</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>設置周期打卡，json</t>
+  </si>
+  <si>
     <t>awark_rule</t>
   </si>
   <si>
-    <t>week_set</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>設置周期打卡，json</t>
-  </si>
-  <si>
-    <t>status_del</t>
-  </si>
-  <si>
-    <t>0--del</t>
-  </si>
-  <si>
-    <t>code</t>
+    <t>time_length</t>
+  </si>
+  <si>
+    <t>時間周期（秒爲單位）</t>
   </si>
   <si>
     <t>log_length</t>
@@ -106,19 +115,16 @@
     <t>獎勵打卡的規則次數</t>
   </si>
   <si>
-    <t>time_length</t>
-  </si>
-  <si>
-    <t>時間周期</t>
-  </si>
-  <si>
     <t>獎勵內容</t>
   </si>
   <si>
-    <t>status_stop</t>
-  </si>
-  <si>
-    <t>0--stop</t>
+    <t>updated_at</t>
+  </si>
+  <si>
+    <t>matter_code</t>
+  </si>
+  <si>
+    <t>提醒任務的類目</t>
   </si>
   <si>
     <t>sign_log 打卡記錄</t>
@@ -136,6 +142,12 @@
     <t>心情類型</t>
   </si>
   <si>
+    <t>action_code</t>
+  </si>
+  <si>
+    <t>活動唯一表示</t>
+  </si>
+  <si>
     <t>year</t>
   </si>
   <si>
@@ -166,28 +178,37 @@
     <t>打卡连击记录数</t>
   </si>
   <si>
-    <t>matter_code</t>
+    <t>crontab_note 定时任务</t>
+  </si>
+  <si>
+    <t>cron_openid</t>
+  </si>
+  <si>
+    <t>json(接受定時任務的用戶)</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>內容</t>
   </si>
   <si>
     <t>json（接受倒计时任务的類目）</t>
   </si>
   <si>
-    <t>crontab_note 定时任务</t>
-  </si>
-  <si>
-    <t>cron_openid</t>
-  </si>
-  <si>
-    <t>json(接受定時任務的用戶)</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>內容</t>
-  </si>
-  <si>
-    <t>days_matter 倒计时人物</t>
+    <t>定時開始時間</t>
+  </si>
+  <si>
+    <t>定時結束時間</t>
+  </si>
+  <si>
+    <t>crontab_time</t>
+  </si>
+  <si>
+    <t>定時時間</t>
+  </si>
+  <si>
+    <t>days_matter 倒计时任務</t>
   </si>
   <si>
     <t>像类似的倒计时记录的log_code也直接合并到这里来</t>
@@ -198,10 +219,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -220,9 +241,64 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -234,28 +310,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -264,6 +318,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -272,6 +333,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,81 +370,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -371,187 +392,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,7 +599,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -615,20 +636,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -644,6 +654,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -667,145 +688,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1140,10 +1161,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="B2:L59"/>
+  <dimension ref="B2:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
@@ -1226,19 +1247,28 @@
       </c>
       <c r="D9" s="2"/>
     </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
     <row r="16" spans="2:12">
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1297,433 +1327,547 @@
     </row>
     <row r="19" spans="2:12">
       <c r="B19" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="G19" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:12">
       <c r="B20" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8">
+        <v>19</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12">
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="2:8">
+        <v>23</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="J21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="2:4">
       <c r="B22" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="2:8">
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="H25" s="2"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="2" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="F27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="6:8">
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
     </row>
     <row r="31" spans="2:4">
-      <c r="B31" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="2"/>
+      <c r="B31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="2:4">
       <c r="B32" s="2" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="2" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" spans="2:4">
       <c r="B34" s="2" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D34" s="2"/>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="2:4">
       <c r="B39" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="C41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="41" spans="2:4">
-      <c r="B41" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" s="2" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="2:4">
-      <c r="B44" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D44" s="2" t="s">
+    <row r="45" spans="2:4">
+      <c r="B45" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="45" spans="2:4">
-      <c r="B45" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
     </row>
     <row r="46" spans="2:4">
       <c r="B46" s="2" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>51</v>
+        <v>5</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="2:4">
+      <c r="B48" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="2:4">
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
+      <c r="C49" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="50" spans="2:4">
       <c r="B50" s="2" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="2:4">
       <c r="B51" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="52" spans="2:4">
       <c r="B52" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="53" spans="2:4">
       <c r="B53" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="54" spans="2:4">
       <c r="B54" s="2" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="55" spans="2:4">
-      <c r="B55" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="2:4">
-      <c r="B56" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="2"/>
-    </row>
     <row r="57" spans="2:4">
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
+      <c r="B57" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
     </row>
     <row r="58" spans="2:4">
       <c r="B58" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="59" spans="2:4">
-      <c r="B59" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
+      <c r="B59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="2:4">
+      <c r="B60" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="2:4">
+      <c r="B61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="2:4">
+      <c r="B62" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="2:4">
+      <c r="B63" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="2:4">
+      <c r="B64" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="2:4">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="2:4">
+      <c r="B66" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="2:4">
+      <c r="B67" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1731,11 +1875,11 @@
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="J16:L16"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B67:D67"/>
     <mergeCell ref="F2:K3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
2017-08-04 23:15:15 everyday last push
</commit_message>
<xml_diff>
--- a/docs/signin_system_dbdisgin.xlsx
+++ b/docs/signin_system_dbdisgin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="10590"/>
+    <workbookView windowWidth="20385" windowHeight="9015"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
     <t>start_time</t>
   </si>
   <si>
-    <t>開始日期</t>
+    <t>開始時間</t>
   </si>
   <si>
     <t>status_del</t>
@@ -85,7 +85,7 @@
     <t>end_time</t>
   </si>
   <si>
-    <t>結束日期</t>
+    <t>結束時間</t>
   </si>
   <si>
     <t>code</t>
@@ -219,10 +219,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -241,7 +241,98 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,69 +347,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -333,8 +361,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -347,35 +376,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -392,13 +392,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,7 +524,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,25 +536,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -452,127 +566,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,6 +591,15 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,26 +628,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -658,6 +658,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -668,165 +683,150 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1163,8 +1163,8 @@
   <sheetPr/>
   <dimension ref="B2:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>

</xml_diff>